<commit_message>
graficos asociados a los datos
</commit_message>
<xml_diff>
--- a/reddit_comentarios_consolidados2.xlsx
+++ b/reddit_comentarios_consolidados2.xlsx
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F2" t="n">
         <v>1</v>
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" t="n">
         <v>2</v>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F5" t="n">
         <v>4</v>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>4</v>
@@ -842,7 +842,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F11" t="n">
         <v>3</v>
@@ -956,7 +956,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="n">
         <v>2</v>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
         <v>2</v>
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F23" t="n">
         <v>2</v>
@@ -1376,7 +1376,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F25" t="n">
         <v>3</v>
@@ -1414,7 +1414,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F26" t="n">
         <v>2</v>
@@ -1719,7 +1719,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F34" t="n">
         <v>1</v>
@@ -1795,7 +1795,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F36" t="n">
         <v>1</v>
@@ -2023,7 +2023,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F42" t="n">
         <v>5</v>
@@ -2219,7 +2219,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F47" t="n">
         <v>1</v>
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F49" t="n">
         <v>2</v>
@@ -2372,7 +2372,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F51" t="n">
         <v>3</v>
@@ -2410,7 +2410,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F52" t="n">
         <v>4</v>
@@ -2448,7 +2448,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F53" t="n">
         <v>2</v>
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="E56" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F56" t="n">
         <v>1</v>
@@ -2600,7 +2600,7 @@
         </is>
       </c>
       <c r="E57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F57" t="n">
         <v>2</v>
@@ -2638,7 +2638,7 @@
         </is>
       </c>
       <c r="E58" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F58" t="n">
         <v>1</v>
@@ -2714,7 +2714,7 @@
         </is>
       </c>
       <c r="E60" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F60" t="n">
         <v>2</v>
@@ -2752,7 +2752,7 @@
         </is>
       </c>
       <c r="E61" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F61" t="n">
         <v>2</v>
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="E69" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F69" t="n">
         <v>1</v>
@@ -3095,7 +3095,7 @@
         </is>
       </c>
       <c r="E70" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F70" t="n">
         <v>1</v>
@@ -3250,7 +3250,7 @@
         </is>
       </c>
       <c r="E74" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F74" t="n">
         <v>1</v>
@@ -3755,7 +3755,7 @@
         </is>
       </c>
       <c r="E87" t="n">
-        <v>-18</v>
+        <v>-17</v>
       </c>
       <c r="F87" t="n">
         <v>1</v>
@@ -3869,7 +3869,7 @@
         </is>
       </c>
       <c r="E90" t="n">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="F90" t="n">
         <v>3</v>
@@ -4211,7 +4211,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>1706</v>
+        <v>1702</v>
       </c>
       <c r="F99" t="n">
         <v>2</v>
@@ -4249,7 +4249,7 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="F100" t="n">
         <v>3</v>
@@ -4287,7 +4287,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="F101" t="n">
         <v>4</v>
@@ -4325,7 +4325,7 @@
         </is>
       </c>
       <c r="E102" t="n">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F102" t="n">
         <v>5</v>
@@ -4401,7 +4401,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F104" t="n">
         <v>7</v>
@@ -4478,7 +4478,7 @@
         </is>
       </c>
       <c r="E106" t="n">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="F106" t="n">
         <v>5</v>
@@ -4554,7 +4554,7 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F108" t="n">
         <v>7</v>
@@ -4593,7 +4593,7 @@
         </is>
       </c>
       <c r="E109" t="n">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F109" t="n">
         <v>8</v>
@@ -4631,7 +4631,7 @@
         </is>
       </c>
       <c r="E110" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F110" t="n">
         <v>9</v>
@@ -4708,7 +4708,7 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F112" t="n">
         <v>8</v>
@@ -4746,7 +4746,7 @@
         </is>
       </c>
       <c r="E113" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F113" t="n">
         <v>9</v>
@@ -4784,7 +4784,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F114" t="n">
         <v>7</v>
@@ -4862,7 +4862,7 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F116" t="n">
         <v>5</v>
@@ -4900,7 +4900,7 @@
         </is>
       </c>
       <c r="E117" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F117" t="n">
         <v>6</v>
@@ -4938,7 +4938,7 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F118" t="n">
         <v>7</v>
@@ -5092,7 +5092,7 @@
         </is>
       </c>
       <c r="E122" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F122" t="n">
         <v>6</v>
@@ -5131,7 +5131,7 @@
         </is>
       </c>
       <c r="E123" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F123" t="n">
         <v>7</v>
@@ -5169,7 +5169,7 @@
         </is>
       </c>
       <c r="E124" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F124" t="n">
         <v>8</v>
@@ -5207,7 +5207,7 @@
         </is>
       </c>
       <c r="E125" t="n">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F125" t="n">
         <v>3</v>
@@ -5283,7 +5283,7 @@
         </is>
       </c>
       <c r="E127" t="n">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F127" t="n">
         <v>5</v>
@@ -5321,7 +5321,7 @@
         </is>
       </c>
       <c r="E128" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F128" t="n">
         <v>6</v>
@@ -5359,7 +5359,7 @@
         </is>
       </c>
       <c r="E129" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F129" t="n">
         <v>7</v>
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="E130" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F130" t="n">
         <v>8</v>
@@ -5435,7 +5435,7 @@
         </is>
       </c>
       <c r="E131" t="n">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F131" t="n">
         <v>2</v>
@@ -5475,7 +5475,7 @@
         </is>
       </c>
       <c r="E132" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F132" t="n">
         <v>3</v>
@@ -5591,7 +5591,7 @@
         </is>
       </c>
       <c r="E135" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F135" t="n">
         <v>4</v>
@@ -5629,7 +5629,7 @@
         </is>
       </c>
       <c r="E136" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F136" t="n">
         <v>4</v>
@@ -5667,7 +5667,7 @@
         </is>
       </c>
       <c r="E137" t="n">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F137" t="n">
         <v>3</v>
@@ -5705,7 +5705,7 @@
         </is>
       </c>
       <c r="E138" t="n">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F138" t="n">
         <v>2</v>
@@ -5744,7 +5744,7 @@
         </is>
       </c>
       <c r="E139" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F139" t="n">
         <v>3</v>
@@ -5782,7 +5782,7 @@
         </is>
       </c>
       <c r="E140" t="n">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F140" t="n">
         <v>4</v>
@@ -5820,7 +5820,7 @@
         </is>
       </c>
       <c r="E141" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F141" t="n">
         <v>5</v>
@@ -5858,7 +5858,7 @@
         </is>
       </c>
       <c r="E142" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F142" t="n">
         <v>6</v>
@@ -5934,7 +5934,7 @@
         </is>
       </c>
       <c r="E144" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F144" t="n">
         <v>4</v>
@@ -5973,7 +5973,7 @@
         </is>
       </c>
       <c r="E145" t="n">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F145" t="n">
         <v>2</v>
@@ -6049,7 +6049,7 @@
         </is>
       </c>
       <c r="E147" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F147" t="n">
         <v>4</v>
@@ -6087,7 +6087,7 @@
         </is>
       </c>
       <c r="E148" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F148" t="n">
         <v>4</v>
@@ -6126,7 +6126,7 @@
         </is>
       </c>
       <c r="E149" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F149" t="n">
         <v>5</v>
@@ -6164,7 +6164,7 @@
         </is>
       </c>
       <c r="E150" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F150" t="n">
         <v>3</v>
@@ -6202,7 +6202,7 @@
         </is>
       </c>
       <c r="E151" t="n">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="F151" t="n">
         <v>2</v>
@@ -6240,7 +6240,7 @@
         </is>
       </c>
       <c r="E152" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F152" t="n">
         <v>3</v>
@@ -6278,7 +6278,7 @@
         </is>
       </c>
       <c r="E153" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F153" t="n">
         <v>3</v>
@@ -6354,7 +6354,7 @@
         </is>
       </c>
       <c r="E155" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F155" t="n">
         <v>2</v>
@@ -6434,7 +6434,7 @@
         </is>
       </c>
       <c r="E157" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F157" t="n">
         <v>3</v>
@@ -6472,7 +6472,7 @@
         </is>
       </c>
       <c r="E158" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F158" t="n">
         <v>2</v>
@@ -6510,7 +6510,7 @@
         </is>
       </c>
       <c r="E159" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F159" t="n">
         <v>2</v>
@@ -6625,7 +6625,7 @@
         </is>
       </c>
       <c r="E162" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F162" t="n">
         <v>5</v>
@@ -6664,7 +6664,7 @@
         </is>
       </c>
       <c r="E163" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F163" t="n">
         <v>4</v>
@@ -6702,7 +6702,7 @@
         </is>
       </c>
       <c r="E164" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F164" t="n">
         <v>2</v>
@@ -6740,7 +6740,7 @@
         </is>
       </c>
       <c r="E165" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F165" t="n">
         <v>2</v>
@@ -6854,7 +6854,7 @@
         </is>
       </c>
       <c r="E168" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F168" t="n">
         <v>3</v>
@@ -6930,7 +6930,7 @@
         </is>
       </c>
       <c r="E170" t="n">
-        <v>934</v>
+        <v>942</v>
       </c>
       <c r="F170" t="n">
         <v>1</v>
@@ -6968,7 +6968,7 @@
         </is>
       </c>
       <c r="E171" t="n">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="F171" t="n">
         <v>2</v>
@@ -7006,7 +7006,7 @@
         </is>
       </c>
       <c r="E172" t="n">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="F172" t="n">
         <v>3</v>
@@ -7044,7 +7044,7 @@
         </is>
       </c>
       <c r="E173" t="n">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F173" t="n">
         <v>2</v>
@@ -7082,7 +7082,7 @@
         </is>
       </c>
       <c r="E174" t="n">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F174" t="n">
         <v>3</v>
@@ -7120,7 +7120,7 @@
         </is>
       </c>
       <c r="E175" t="n">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F175" t="n">
         <v>4</v>
@@ -7159,7 +7159,7 @@
         </is>
       </c>
       <c r="E176" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F176" t="n">
         <v>5</v>
@@ -7235,7 +7235,7 @@
         </is>
       </c>
       <c r="E178" t="n">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F178" t="n">
         <v>5</v>
@@ -7273,7 +7273,7 @@
         </is>
       </c>
       <c r="E179" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F179" t="n">
         <v>4</v>
@@ -7311,7 +7311,7 @@
         </is>
       </c>
       <c r="E180" t="n">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F180" t="n">
         <v>4</v>
@@ -7349,7 +7349,7 @@
         </is>
       </c>
       <c r="E181" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F181" t="n">
         <v>5</v>
@@ -7387,7 +7387,7 @@
         </is>
       </c>
       <c r="E182" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F182" t="n">
         <v>6</v>
@@ -7425,7 +7425,7 @@
         </is>
       </c>
       <c r="E183" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F183" t="n">
         <v>4</v>
@@ -7463,7 +7463,7 @@
         </is>
       </c>
       <c r="E184" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F184" t="n">
         <v>4</v>
@@ -7501,7 +7501,7 @@
         </is>
       </c>
       <c r="E185" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F185" t="n">
         <v>4</v>
@@ -7539,7 +7539,7 @@
         </is>
       </c>
       <c r="E186" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F186" t="n">
         <v>4</v>
@@ -7578,7 +7578,7 @@
         </is>
       </c>
       <c r="E187" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F187" t="n">
         <v>4</v>
@@ -7617,7 +7617,7 @@
         </is>
       </c>
       <c r="E188" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F188" t="n">
         <v>4</v>
@@ -7655,7 +7655,7 @@
         </is>
       </c>
       <c r="E189" t="n">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="F189" t="n">
         <v>1</v>
@@ -7693,7 +7693,7 @@
         </is>
       </c>
       <c r="E190" t="n">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="F190" t="n">
         <v>2</v>
@@ -7731,7 +7731,7 @@
         </is>
       </c>
       <c r="E191" t="n">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="F191" t="n">
         <v>3</v>
@@ -7809,7 +7809,7 @@
         </is>
       </c>
       <c r="E193" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F193" t="n">
         <v>5</v>
@@ -7848,7 +7848,7 @@
         </is>
       </c>
       <c r="E194" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F194" t="n">
         <v>6</v>
@@ -7887,7 +7887,7 @@
         </is>
       </c>
       <c r="E195" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F195" t="n">
         <v>7</v>
@@ -8043,7 +8043,7 @@
         </is>
       </c>
       <c r="E199" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F199" t="n">
         <v>3</v>
@@ -8119,7 +8119,7 @@
         </is>
       </c>
       <c r="E201" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F201" t="n">
         <v>4</v>
@@ -8197,7 +8197,7 @@
         </is>
       </c>
       <c r="E203" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F203" t="n">
         <v>2</v>
@@ -8237,7 +8237,7 @@
         </is>
       </c>
       <c r="E204" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F204" t="n">
         <v>3</v>
@@ -8275,7 +8275,7 @@
         </is>
       </c>
       <c r="E205" t="n">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="F205" t="n">
         <v>3</v>
@@ -8314,7 +8314,7 @@
         </is>
       </c>
       <c r="E206" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F206" t="n">
         <v>4</v>
@@ -8352,7 +8352,7 @@
         </is>
       </c>
       <c r="E207" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F207" t="n">
         <v>2</v>
@@ -8391,7 +8391,7 @@
         </is>
       </c>
       <c r="E208" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F208" t="n">
         <v>3</v>
@@ -8429,7 +8429,7 @@
         </is>
       </c>
       <c r="E209" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F209" t="n">
         <v>3</v>
@@ -8513,7 +8513,7 @@
         </is>
       </c>
       <c r="E211" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F211" t="n">
         <v>2</v>
@@ -8551,7 +8551,7 @@
         </is>
       </c>
       <c r="E212" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F212" t="n">
         <v>2</v>
@@ -8590,7 +8590,7 @@
         </is>
       </c>
       <c r="E213" t="n">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F213" t="n">
         <v>1</v>
@@ -8629,7 +8629,7 @@
         </is>
       </c>
       <c r="E214" t="n">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F214" t="n">
         <v>2</v>
@@ -8669,7 +8669,7 @@
         </is>
       </c>
       <c r="E215" t="n">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F215" t="n">
         <v>3</v>
@@ -8707,7 +8707,7 @@
         </is>
       </c>
       <c r="E216" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F216" t="n">
         <v>4</v>
@@ -8745,7 +8745,7 @@
         </is>
       </c>
       <c r="E217" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F217" t="n">
         <v>5</v>
@@ -8821,7 +8821,7 @@
         </is>
       </c>
       <c r="E219" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F219" t="n">
         <v>5</v>
@@ -8859,7 +8859,7 @@
         </is>
       </c>
       <c r="E220" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F220" t="n">
         <v>6</v>
@@ -8897,7 +8897,7 @@
         </is>
       </c>
       <c r="E221" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F221" t="n">
         <v>4</v>
@@ -9011,7 +9011,7 @@
         </is>
       </c>
       <c r="E224" t="n">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F224" t="n">
         <v>1</v>
@@ -9051,7 +9051,7 @@
         </is>
       </c>
       <c r="E225" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F225" t="n">
         <v>2</v>
@@ -9090,7 +9090,7 @@
         </is>
       </c>
       <c r="E226" t="n">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F226" t="n">
         <v>1</v>
@@ -9128,7 +9128,7 @@
         </is>
       </c>
       <c r="E227" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F227" t="n">
         <v>2</v>
@@ -9204,7 +9204,7 @@
         </is>
       </c>
       <c r="E229" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F229" t="n">
         <v>4</v>
@@ -9242,7 +9242,7 @@
         </is>
       </c>
       <c r="E230" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F230" t="n">
         <v>5</v>
@@ -9280,7 +9280,7 @@
         </is>
       </c>
       <c r="E231" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F231" t="n">
         <v>6</v>
@@ -9356,7 +9356,7 @@
         </is>
       </c>
       <c r="E233" t="n">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F233" t="n">
         <v>2</v>
@@ -9395,7 +9395,7 @@
         </is>
       </c>
       <c r="E234" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F234" t="n">
         <v>3</v>
@@ -9433,7 +9433,7 @@
         </is>
       </c>
       <c r="E235" t="n">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="F235" t="n">
         <v>1</v>
@@ -9510,7 +9510,7 @@
         </is>
       </c>
       <c r="E237" t="n">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F237" t="n">
         <v>2</v>
@@ -9548,7 +9548,7 @@
         </is>
       </c>
       <c r="E238" t="n">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="F238" t="n">
         <v>3</v>
@@ -9586,7 +9586,7 @@
         </is>
       </c>
       <c r="E239" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F239" t="n">
         <v>4</v>
@@ -9624,7 +9624,7 @@
         </is>
       </c>
       <c r="E240" t="n">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F240" t="n">
         <v>3</v>
@@ -9662,7 +9662,7 @@
         </is>
       </c>
       <c r="E241" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F241" t="n">
         <v>4</v>
@@ -9700,7 +9700,7 @@
         </is>
       </c>
       <c r="E242" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F242" t="n">
         <v>2</v>
@@ -9738,7 +9738,7 @@
         </is>
       </c>
       <c r="E243" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F243" t="n">
         <v>1</v>
@@ -9814,7 +9814,7 @@
         </is>
       </c>
       <c r="E245" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F245" t="n">
         <v>3</v>
@@ -9852,7 +9852,7 @@
         </is>
       </c>
       <c r="E246" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F246" t="n">
         <v>4</v>
@@ -9890,7 +9890,7 @@
         </is>
       </c>
       <c r="E247" t="n">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F247" t="n">
         <v>3</v>
@@ -9928,7 +9928,7 @@
         </is>
       </c>
       <c r="E248" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F248" t="n">
         <v>4</v>
@@ -9966,7 +9966,7 @@
         </is>
       </c>
       <c r="E249" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F249" t="n">
         <v>5</v>
@@ -10005,7 +10005,7 @@
         </is>
       </c>
       <c r="E250" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F250" t="n">
         <v>5</v>
@@ -10082,7 +10082,7 @@
         </is>
       </c>
       <c r="E252" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F252" t="n">
         <v>3</v>
@@ -10120,7 +10120,7 @@
         </is>
       </c>
       <c r="E253" t="n">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F253" t="n">
         <v>1</v>
@@ -10158,7 +10158,7 @@
         </is>
       </c>
       <c r="E254" t="n">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F254" t="n">
         <v>2</v>
@@ -10234,7 +10234,7 @@
         </is>
       </c>
       <c r="E256" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F256" t="n">
         <v>2</v>
@@ -10274,7 +10274,7 @@
         </is>
       </c>
       <c r="E257" t="n">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F257" t="n">
         <v>1</v>
@@ -10312,7 +10312,7 @@
         </is>
       </c>
       <c r="E258" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F258" t="n">
         <v>2</v>
@@ -10350,7 +10350,7 @@
         </is>
       </c>
       <c r="E259" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F259" t="n">
         <v>3</v>
@@ -10428,7 +10428,7 @@
         </is>
       </c>
       <c r="E261" t="n">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F261" t="n">
         <v>2</v>
@@ -10466,7 +10466,7 @@
         </is>
       </c>
       <c r="E262" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F262" t="n">
         <v>3</v>
@@ -10505,7 +10505,7 @@
         </is>
       </c>
       <c r="E263" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F263" t="n">
         <v>2</v>
@@ -10581,7 +10581,7 @@
         </is>
       </c>
       <c r="E265" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F265" t="n">
         <v>1</v>
@@ -10620,7 +10620,7 @@
         </is>
       </c>
       <c r="E266" t="n">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F266" t="n">
         <v>2</v>
@@ -10696,7 +10696,7 @@
         </is>
       </c>
       <c r="E268" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F268" t="n">
         <v>4</v>
@@ -10773,7 +10773,7 @@
         </is>
       </c>
       <c r="E270" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F270" t="n">
         <v>1</v>
@@ -10811,7 +10811,7 @@
         </is>
       </c>
       <c r="E271" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F271" t="n">
         <v>2</v>
@@ -10849,7 +10849,7 @@
         </is>
       </c>
       <c r="E272" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F272" t="n">
         <v>3</v>
@@ -10887,7 +10887,7 @@
         </is>
       </c>
       <c r="E273" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F273" t="n">
         <v>3</v>
@@ -10925,7 +10925,7 @@
         </is>
       </c>
       <c r="E274" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F274" t="n">
         <v>4</v>
@@ -10963,7 +10963,7 @@
         </is>
       </c>
       <c r="E275" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F275" t="n">
         <v>5</v>
@@ -11040,7 +11040,7 @@
         </is>
       </c>
       <c r="E277" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F277" t="n">
         <v>3</v>
@@ -11116,7 +11116,7 @@
         </is>
       </c>
       <c r="E279" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F279" t="n">
         <v>1</v>
@@ -11154,7 +11154,7 @@
         </is>
       </c>
       <c r="E280" t="n">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F280" t="n">
         <v>2</v>
@@ -11192,7 +11192,7 @@
         </is>
       </c>
       <c r="E281" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F281" t="n">
         <v>2</v>
@@ -11230,7 +11230,7 @@
         </is>
       </c>
       <c r="E282" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F282" t="n">
         <v>2</v>
@@ -11268,7 +11268,7 @@
         </is>
       </c>
       <c r="E283" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F283" t="n">
         <v>2</v>
@@ -11345,7 +11345,7 @@
         </is>
       </c>
       <c r="E285" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F285" t="n">
         <v>1</v>
@@ -11383,7 +11383,7 @@
         </is>
       </c>
       <c r="E286" t="n">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F286" t="n">
         <v>2</v>
@@ -11423,7 +11423,7 @@
         </is>
       </c>
       <c r="E287" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F287" t="n">
         <v>2</v>
@@ -11462,7 +11462,7 @@
         </is>
       </c>
       <c r="E288" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F288" t="n">
         <v>1</v>
@@ -11500,7 +11500,7 @@
         </is>
       </c>
       <c r="E289" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F289" t="n">
         <v>1</v>
@@ -11541,7 +11541,7 @@
         </is>
       </c>
       <c r="E290" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F290" t="n">
         <v>2</v>
@@ -11579,7 +11579,7 @@
         </is>
       </c>
       <c r="E291" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F291" t="n">
         <v>2</v>
@@ -11617,7 +11617,7 @@
         </is>
       </c>
       <c r="E292" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F292" t="n">
         <v>1</v>
@@ -11694,7 +11694,7 @@
         </is>
       </c>
       <c r="E294" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F294" t="n">
         <v>1</v>
@@ -11889,7 +11889,7 @@
         </is>
       </c>
       <c r="E299" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F299" t="n">
         <v>2</v>
@@ -12042,7 +12042,7 @@
         </is>
       </c>
       <c r="E303" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F303" t="n">
         <v>1</v>
@@ -12120,7 +12120,7 @@
         </is>
       </c>
       <c r="E305" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F305" t="n">
         <v>1</v>
@@ -12388,7 +12388,7 @@
         </is>
       </c>
       <c r="E312" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F312" t="n">
         <v>1</v>
@@ -12502,7 +12502,7 @@
         </is>
       </c>
       <c r="E315" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F315" t="n">
         <v>4</v>
@@ -12654,7 +12654,7 @@
         </is>
       </c>
       <c r="E319" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F319" t="n">
         <v>1</v>
@@ -13193,7 +13193,7 @@
         </is>
       </c>
       <c r="E333" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F333" t="n">
         <v>4</v>
@@ -13539,7 +13539,7 @@
         </is>
       </c>
       <c r="E342" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F342" t="n">
         <v>3</v>
@@ -13654,7 +13654,7 @@
         </is>
       </c>
       <c r="E345" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F345" t="n">
         <v>3</v>
@@ -13776,7 +13776,7 @@
         </is>
       </c>
       <c r="E348" t="n">
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="F348" t="n">
         <v>6</v>
@@ -13967,7 +13967,7 @@
         </is>
       </c>
       <c r="E353" t="n">
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="F353" t="n">
         <v>6</v>
@@ -14005,7 +14005,7 @@
         </is>
       </c>
       <c r="E354" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F354" t="n">
         <v>7</v>
@@ -14312,7 +14312,7 @@
         </is>
       </c>
       <c r="E362" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F362" t="n">
         <v>4</v>
@@ -14350,7 +14350,7 @@
         </is>
       </c>
       <c r="E363" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F363" t="n">
         <v>1</v>
@@ -14503,7 +14503,7 @@
         </is>
       </c>
       <c r="E367" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F367" t="n">
         <v>1</v>
@@ -14541,7 +14541,7 @@
         </is>
       </c>
       <c r="E368" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F368" t="n">
         <v>2</v>
@@ -14733,7 +14733,7 @@
         </is>
       </c>
       <c r="E373" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F373" t="n">
         <v>7</v>
@@ -14886,7 +14886,7 @@
         </is>
       </c>
       <c r="E377" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F377" t="n">
         <v>4</v>
@@ -14927,7 +14927,7 @@
         </is>
       </c>
       <c r="E378" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F378" t="n">
         <v>5</v>
@@ -15234,7 +15234,7 @@
         </is>
       </c>
       <c r="E386" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F386" t="n">
         <v>2</v>
@@ -15272,7 +15272,7 @@
         </is>
       </c>
       <c r="E387" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F387" t="n">
         <v>1</v>
@@ -15310,7 +15310,7 @@
         </is>
       </c>
       <c r="E388" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F388" t="n">
         <v>1</v>
@@ -15425,7 +15425,7 @@
         </is>
       </c>
       <c r="E391" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F391" t="n">
         <v>4</v>
@@ -15657,7 +15657,7 @@
         </is>
       </c>
       <c r="E397" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F397" t="n">
         <v>1</v>
@@ -15811,7 +15811,7 @@
         </is>
       </c>
       <c r="E401" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F401" t="n">
         <v>1</v>
@@ -15849,7 +15849,7 @@
         </is>
       </c>
       <c r="E402" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F402" t="n">
         <v>2</v>
@@ -16317,7 +16317,7 @@
         </is>
       </c>
       <c r="E414" t="n">
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="F414" t="n">
         <v>3</v>
@@ -16355,7 +16355,7 @@
         </is>
       </c>
       <c r="E415" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F415" t="n">
         <v>4</v>
@@ -16431,7 +16431,7 @@
         </is>
       </c>
       <c r="E417" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F417" t="n">
         <v>2</v>
@@ -16697,7 +16697,7 @@
         </is>
       </c>
       <c r="E424" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F424" t="n">
         <v>4</v>
@@ -16773,7 +16773,7 @@
         </is>
       </c>
       <c r="E426" t="n">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F426" t="n">
         <v>1</v>
@@ -16811,7 +16811,7 @@
         </is>
       </c>
       <c r="E427" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F427" t="n">
         <v>2</v>
@@ -16849,7 +16849,7 @@
         </is>
       </c>
       <c r="E428" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F428" t="n">
         <v>2</v>
@@ -16888,7 +16888,7 @@
         </is>
       </c>
       <c r="E429" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F429" t="n">
         <v>2</v>
@@ -16928,7 +16928,7 @@
         </is>
       </c>
       <c r="E430" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F430" t="n">
         <v>3</v>
@@ -16966,7 +16966,7 @@
         </is>
       </c>
       <c r="E431" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F431" t="n">
         <v>2</v>
@@ -17123,7 +17123,7 @@
         </is>
       </c>
       <c r="E435" t="n">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F435" t="n">
         <v>1</v>
@@ -17431,7 +17431,7 @@
         </is>
       </c>
       <c r="E443" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F443" t="n">
         <v>1</v>
@@ -17470,7 +17470,7 @@
         </is>
       </c>
       <c r="E444" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F444" t="n">
         <v>2</v>
@@ -17510,7 +17510,7 @@
         </is>
       </c>
       <c r="E445" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F445" t="n">
         <v>1</v>
@@ -17627,7 +17627,7 @@
         </is>
       </c>
       <c r="E448" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F448" t="n">
         <v>2</v>
@@ -17665,7 +17665,7 @@
         </is>
       </c>
       <c r="E449" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F449" t="n">
         <v>1</v>
@@ -17703,7 +17703,7 @@
         </is>
       </c>
       <c r="E450" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F450" t="n">
         <v>2</v>
@@ -17973,7 +17973,7 @@
         </is>
       </c>
       <c r="E457" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F457" t="n">
         <v>1</v>
@@ -18050,7 +18050,7 @@
         </is>
       </c>
       <c r="E459" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F459" t="n">
         <v>1</v>
@@ -18088,7 +18088,7 @@
         </is>
       </c>
       <c r="E460" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F460" t="n">
         <v>2</v>
@@ -18164,7 +18164,7 @@
         </is>
       </c>
       <c r="E462" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F462" t="n">
         <v>1</v>
@@ -18204,7 +18204,7 @@
         </is>
       </c>
       <c r="E463" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F463" t="n">
         <v>1</v>
@@ -18242,7 +18242,7 @@
         </is>
       </c>
       <c r="E464" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F464" t="n">
         <v>2</v>
@@ -18403,7 +18403,7 @@
         </is>
       </c>
       <c r="E468" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F468" t="n">
         <v>1</v>
@@ -18519,7 +18519,7 @@
         </is>
       </c>
       <c r="E471" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F471" t="n">
         <v>2</v>
@@ -18559,7 +18559,7 @@
         </is>
       </c>
       <c r="E472" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F472" t="n">
         <v>3</v>
@@ -18829,7 +18829,7 @@
         </is>
       </c>
       <c r="E479" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F479" t="n">
         <v>1</v>
@@ -18906,7 +18906,7 @@
         </is>
       </c>
       <c r="E481" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F481" t="n">
         <v>1</v>
@@ -18982,7 +18982,7 @@
         </is>
       </c>
       <c r="E483" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F483" t="n">
         <v>3</v>
@@ -19252,7 +19252,7 @@
         </is>
       </c>
       <c r="E490" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F490" t="n">
         <v>1</v>
@@ -19342,7 +19342,7 @@
         </is>
       </c>
       <c r="E492" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F492" t="n">
         <v>1</v>
@@ -19536,7 +19536,7 @@
         </is>
       </c>
       <c r="E497" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F497" t="n">
         <v>1</v>
@@ -19613,7 +19613,7 @@
         </is>
       </c>
       <c r="E499" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F499" t="n">
         <v>3</v>
@@ -21080,7 +21080,7 @@
         </is>
       </c>
       <c r="E537" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F537" t="n">
         <v>2</v>
@@ -21157,7 +21157,7 @@
         </is>
       </c>
       <c r="E539" t="n">
-        <v>-4</v>
+        <v>-5</v>
       </c>
       <c r="F539" t="n">
         <v>1</v>
@@ -21311,7 +21311,7 @@
         </is>
       </c>
       <c r="E543" t="n">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="F543" t="n">
         <v>1</v>
@@ -21744,7 +21744,7 @@
         </is>
       </c>
       <c r="E554" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F554" t="n">
         <v>1</v>
@@ -21820,7 +21820,7 @@
         </is>
       </c>
       <c r="E556" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F556" t="n">
         <v>1</v>
@@ -21935,7 +21935,7 @@
         </is>
       </c>
       <c r="E559" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F559" t="n">
         <v>1</v>
@@ -22091,7 +22091,7 @@
         </is>
       </c>
       <c r="E563" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F563" t="n">
         <v>1</v>
@@ -22673,7 +22673,7 @@
         </is>
       </c>
       <c r="E578" t="n">
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="F578" t="n">
         <v>1</v>
@@ -22787,7 +22787,7 @@
         </is>
       </c>
       <c r="E581" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F581" t="n">
         <v>2</v>
@@ -22825,7 +22825,7 @@
         </is>
       </c>
       <c r="E582" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F582" t="n">
         <v>1</v>
@@ -22863,7 +22863,7 @@
         </is>
       </c>
       <c r="E583" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F583" t="n">
         <v>2</v>
@@ -22939,7 +22939,7 @@
         </is>
       </c>
       <c r="E585" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F585" t="n">
         <v>3</v>
@@ -22977,7 +22977,7 @@
         </is>
       </c>
       <c r="E586" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F586" t="n">
         <v>4</v>
@@ -23053,7 +23053,7 @@
         </is>
       </c>
       <c r="E588" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F588" t="n">
         <v>6</v>
@@ -23129,7 +23129,7 @@
         </is>
       </c>
       <c r="E590" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F590" t="n">
         <v>8</v>
@@ -23205,7 +23205,7 @@
         </is>
       </c>
       <c r="E592" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F592" t="n">
         <v>3</v>
@@ -23359,7 +23359,7 @@
         </is>
       </c>
       <c r="E596" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F596" t="n">
         <v>1</v>
@@ -23435,7 +23435,7 @@
         </is>
       </c>
       <c r="E598" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F598" t="n">
         <v>3</v>
@@ -23626,7 +23626,7 @@
         </is>
       </c>
       <c r="E603" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F603" t="n">
         <v>1</v>
@@ -23740,7 +23740,7 @@
         </is>
       </c>
       <c r="E606" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F606" t="n">
         <v>1</v>
@@ -24013,7 +24013,7 @@
         </is>
       </c>
       <c r="E613" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F613" t="n">
         <v>1</v>
@@ -24052,7 +24052,7 @@
         </is>
       </c>
       <c r="E614" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F614" t="n">
         <v>2</v>
@@ -24130,7 +24130,7 @@
         </is>
       </c>
       <c r="E616" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F616" t="n">
         <v>4</v>
@@ -24174,7 +24174,7 @@
         </is>
       </c>
       <c r="E617" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F617" t="n">
         <v>5</v>

</xml_diff>